<commit_message>
fix twilio config eror
</commit_message>
<xml_diff>
--- a/scripts/fitness_tracker_dataset.xlsx
+++ b/scripts/fitness_tracker_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\owencooke15\projects\uaec-2024\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F14FA4-C66C-4BAE-AF59-760B1CB1041A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3339434-01BF-4268-AB79-20E00F9307D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5CAFEF88-F8FE-4309-8487-A1508297C9B1}"/>
   </bookViews>
@@ -489,7 +489,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,7 +809,7 @@
         <v>45598</v>
       </c>
       <c r="C9">
-        <v>4318</v>
+        <v>14318</v>
       </c>
       <c r="D9">
         <v>1628.86</v>

</xml_diff>